<commit_message>
Add chache baremetal explanation to main README
</commit_message>
<xml_diff>
--- a/results/CycloneVSoC_baremetal_cache.xlsx
+++ b/results/CycloneVSoC_baremetal_cache.xlsx
@@ -867,11 +867,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="208547840"/>
-        <c:axId val="145449536"/>
+        <c:axId val="210615296"/>
+        <c:axId val="147873792"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="208547840"/>
+        <c:axId val="210615296"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -881,7 +881,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="145449536"/>
+        <c:crossAx val="147873792"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -889,7 +889,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="145449536"/>
+        <c:axId val="147873792"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -919,7 +919,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="208547840"/>
+        <c:crossAx val="210615296"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -977,19 +977,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_7" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_16" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_14" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_12" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_10" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_4" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable12.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_12" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_5" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable13.xml><?xml version="1.0" encoding="utf-8"?>
@@ -997,19 +997,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable14.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_16" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_15" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_6" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_5" connectionId="11" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_2" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_14" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1017,19 +1017,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_10" connectionId="16" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_8" connectionId="14" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_4" connectionId="10" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_0" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_7" connectionId="13" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_6" connectionId="12" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="Cache_15" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -9976,7 +9976,7 @@
   <dimension ref="A1:AE26"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P42" sqref="P42"/>
+      <selection activeCell="H26" sqref="H26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>